<commit_message>
Added graphs for fun.
</commit_message>
<xml_diff>
--- a/Recorded Data/FinalData.xlsx
+++ b/Recorded Data/FinalData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="learning.csv" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -181,7 +181,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -234,8 +234,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -254,7 +254,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:yVal>
             <c:numRef>
               <c:f>learning.csv!$I$2:$I$69</c:f>
               <c:numCache>
@@ -466,8 +466,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -486,7 +486,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:yVal>
             <c:numRef>
               <c:f>learning.csv!$J$2:$J$69</c:f>
               <c:numCache>
@@ -698,8 +698,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -718,7 +718,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:yVal>
             <c:numRef>
               <c:f>learning.csv!$K$2:$K$69</c:f>
               <c:numCache>
@@ -930,8 +930,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -941,13 +941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2118674984"/>
-        <c:axId val="-2117196216"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-2118674984"/>
+        <c:axId val="2125023304"/>
+        <c:axId val="2124150376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2125023304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -980,15 +978,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117196216"/>
+        <c:crossAx val="2124150376"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="-2117196216"/>
+        <c:axId val="2124150376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,9 +1013,9 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118674984"/>
+        <c:crossAx val="2125023304"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1302,11 +1297,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2120904552"/>
-        <c:axId val="-2120663016"/>
+        <c:axId val="2124215192"/>
+        <c:axId val="2124220664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120904552"/>
+        <c:axId val="2124215192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +1329,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120663016"/>
+        <c:crossAx val="2124220664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1342,7 +1337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120663016"/>
+        <c:axId val="2124220664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120904552"/>
+        <c:crossAx val="2124215192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1398,16 +1393,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1783,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX11999"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AC43" sqref="AC43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1871,15 +1866,15 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <f ca="1">AVERAGE(OFFSET($G$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f ca="1">AVERAGE(OFFSET($G$2,(ROW()-ROW($J$2))*173,,173,))</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f ca="1">AVERAGE(OFFSET($F$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f ca="1">AVERAGE(OFFSET($F$2,(ROW()-ROW($K$2))*173,,173,))</f>
         <v>0.12138728323699421</v>
       </c>
       <c r="L2">
-        <f>AVERAGE(A2:E2)</f>
+        <f t="shared" ref="L2:L33" si="0">AVERAGE(A2:E2)</f>
         <v>1.4</v>
       </c>
       <c r="N2">
@@ -1927,19 +1922,19 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" ca="1" si="0">AVERAGE(OFFSET($H$2,(ROW()-ROW($I$2))*30,,30,))</f>
+        <f t="shared" ref="I3:I66" ca="1" si="1">AVERAGE(OFFSET($H$2,(ROW()-ROW($I$2))*30,,30,))</f>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J66" ca="1" si="1">AVERAGE(OFFSET($G$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ref="J3:J66" ca="1" si="2">AVERAGE(OFFSET($G$2,(ROW()-ROW($J$2))*173,,173,))</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K66" ca="1" si="2">AVERAGE(OFFSET($F$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ref="K3:K66" ca="1" si="3">AVERAGE(OFFSET($F$2,(ROW()-ROW($K$2))*173,,173,))</f>
         <v>0.20809248554913296</v>
       </c>
       <c r="L3">
-        <f>AVERAGE(A3:E3)</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="N3">
@@ -1990,19 +1985,19 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.10404624277456648</v>
       </c>
       <c r="L4">
-        <f>AVERAGE(A4:E4)</f>
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="N4">
@@ -2053,19 +2048,19 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0.10404624277456648</v>
       </c>
       <c r="K5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>7.5144508670520235E-2</v>
       </c>
       <c r="L5">
-        <f>AVERAGE(A5:E5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N5">
@@ -2116,19 +2111,19 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.2023121387283239E-2</v>
       </c>
       <c r="K6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>6.358381502890173E-2</v>
       </c>
       <c r="L6">
-        <f>AVERAGE(A6:E6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N6">
@@ -2178,19 +2173,19 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="K7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>6.9364161849710976E-2</v>
       </c>
       <c r="L7">
-        <f>AVERAGE(A7:E7)</f>
+        <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
       <c r="N7">
@@ -2240,19 +2235,19 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="K8">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="L8">
-        <f>AVERAGE(A8:E8)</f>
+        <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
       <c r="N8">
@@ -2302,19 +2297,19 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>6.358381502890173E-2</v>
       </c>
       <c r="K9">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L9">
-        <f>AVERAGE(A9:E9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N9">
@@ -2350,19 +2345,19 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="J10">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="K10">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="L10">
-        <f>AVERAGE(A10:E10)</f>
+        <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
       <c r="N10">
@@ -2398,19 +2393,19 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.7803468208092484E-2</v>
       </c>
       <c r="K11">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L11">
-        <f>AVERAGE(A11:E11)</f>
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="N11">
@@ -2446,19 +2441,19 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="L12">
-        <f>AVERAGE(A12:E12)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="M12" s="1"/>
@@ -2530,67 +2525,67 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J13">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.3121387283236993E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.4682080924855488E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3121387283236993E-2</v>
-      </c>
-      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
-      <c r="L13">
-        <f>AVERAGE(A13:E13)</f>
-        <v>3.2</v>
-      </c>
-      <c r="N13">
-        <v>4</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:50">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.4682080924855488E-2</v>
-      </c>
       <c r="K14">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L14">
-        <f>AVERAGE(A14:E14)</f>
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="N14">
@@ -2626,19 +2621,19 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J15">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L15">
-        <f>AVERAGE(A15:E15)</f>
+        <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
       <c r="N15">
@@ -2674,19 +2669,19 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J16">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="K16">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="L16">
-        <f>AVERAGE(A16:E16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N16">
@@ -2722,19 +2717,19 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="J17">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L17">
-        <f>AVERAGE(A17:E17)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="N17">
@@ -2770,67 +2765,67 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J18">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.8901734104046242E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.046242774566474E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="N18">
+        <v>14</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8901734104046242E-2</v>
-      </c>
-      <c r="K18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J19">
         <f t="shared" ca="1" si="2"/>
         <v>4.046242774566474E-2</v>
       </c>
-      <c r="L18">
-        <f>AVERAGE(A18:E18)</f>
-        <v>1.4</v>
-      </c>
-      <c r="N18">
-        <v>14</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="J19">
-        <f t="shared" ca="1" si="1"/>
+      <c r="K19">
+        <f t="shared" ca="1" si="3"/>
         <v>4.046242774566474E-2</v>
       </c>
-      <c r="K19">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.046242774566474E-2</v>
-      </c>
       <c r="L19">
-        <f>AVERAGE(A19:E19)</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="N19">
@@ -2866,19 +2861,19 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J20">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K20">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="L20">
-        <f>AVERAGE(A20:E20)</f>
+        <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
       <c r="N20">
@@ -2914,19 +2909,19 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="L21">
-        <f>AVERAGE(A21:E21)</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="N21">
@@ -2960,19 +2955,19 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J22">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1560693641618497E-2</v>
-      </c>
-      <c r="K22">
         <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
+      <c r="K22">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.1560693641618497E-2</v>
+      </c>
       <c r="L22">
-        <f>AVERAGE(A22:E22)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="N22">
@@ -3006,19 +3001,19 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="J23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L23">
-        <f>AVERAGE(A23:E23)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N23">
@@ -3052,19 +3047,19 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="J24">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L24">
-        <f>AVERAGE(A24:E24)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
       <c r="N24">
@@ -3098,19 +3093,19 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.3</v>
       </c>
       <c r="J25">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="K25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="L25">
-        <f>AVERAGE(A25:E25)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="N25">
@@ -3144,19 +3139,19 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.36666666666666664</v>
       </c>
       <c r="J26">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K26">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L26">
-        <f>AVERAGE(A26:E26)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="N26">
@@ -3190,19 +3185,19 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J27">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K27">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L27">
-        <f>AVERAGE(A27:E27)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="N27">
@@ -3236,19 +3231,19 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.43333333333333335</v>
       </c>
       <c r="J28">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.7341040462427744E-2</v>
-      </c>
-      <c r="K28">
         <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
+      <c r="K28">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.7341040462427744E-2</v>
+      </c>
       <c r="L28">
-        <f>AVERAGE(A28:E28)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="N28">
@@ -3282,19 +3277,19 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.43333333333333335</v>
       </c>
       <c r="J29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K29">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="L29">
-        <f>AVERAGE(A29:E29)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="N29">
@@ -3328,19 +3323,19 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="J30">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="K30">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L30">
-        <f>AVERAGE(A30:E30)</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
       <c r="N30">
@@ -3374,19 +3369,19 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J31">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.3121387283236993E-2</v>
-      </c>
-      <c r="K31">
         <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
+      <c r="K31">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.3121387283236993E-2</v>
+      </c>
       <c r="L31">
-        <f>AVERAGE(A31:E31)</f>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
       <c r="N31">
@@ -3416,19 +3411,19 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J32">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="K32">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L32">
-        <f>AVERAGE(A32:E32)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N32">
@@ -3458,19 +3453,19 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J33">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K33">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L33">
-        <f>AVERAGE(A33:E33)</f>
+        <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="N33">
@@ -3500,19 +3495,19 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="K34">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="L34">
-        <f>AVERAGE(A34:E34)</f>
+        <f t="shared" ref="L34:L69" si="4">AVERAGE(A34:E34)</f>
         <v>3.6666666666666665</v>
       </c>
       <c r="N34">
@@ -3542,19 +3537,19 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.2</v>
       </c>
       <c r="J35">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="K35">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L35">
-        <f>AVERAGE(A35:E35)</f>
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="N35">
@@ -3584,19 +3579,19 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.23333333333333334</v>
       </c>
       <c r="J36">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="K36">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="L36">
-        <f>AVERAGE(A36:E36)</f>
+        <f t="shared" si="4"/>
         <v>6.666666666666667</v>
       </c>
       <c r="N36">
@@ -3626,19 +3621,19 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.36666666666666664</v>
       </c>
       <c r="J37">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="K37">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="L37">
-        <f>AVERAGE(A37:E37)</f>
+        <f t="shared" si="4"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="N37">
@@ -3668,19 +3663,19 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.43333333333333335</v>
       </c>
       <c r="J38">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.4682080924855488E-2</v>
-      </c>
-      <c r="K38">
         <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
+      <c r="K38">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.4682080924855488E-2</v>
+      </c>
       <c r="L38">
-        <f>AVERAGE(A38:E38)</f>
+        <f t="shared" si="4"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="N38">
@@ -3710,19 +3705,19 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.5</v>
       </c>
       <c r="J39">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="K39">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L39">
-        <f>AVERAGE(A39:E39)</f>
+        <f t="shared" si="4"/>
         <v>4.666666666666667</v>
       </c>
       <c r="N39">
@@ -3752,19 +3747,19 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.3</v>
       </c>
       <c r="J40">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K40">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="L40">
-        <f>AVERAGE(A40:E40)</f>
+        <f t="shared" si="4"/>
         <v>7.333333333333333</v>
       </c>
       <c r="N40">
@@ -3794,19 +3789,19 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="J41">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K41">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.2023121387283239E-2</v>
       </c>
       <c r="L41">
-        <f>AVERAGE(A41:E41)</f>
+        <f t="shared" si="4"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="N41">
@@ -3836,19 +3831,19 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="J42">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="K42">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="L42">
-        <f>AVERAGE(A42:E42)</f>
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="N42">
@@ -3878,19 +3873,19 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.9</v>
       </c>
       <c r="J43">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.2023121387283239E-2</v>
       </c>
       <c r="K43">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="L43">
-        <f>AVERAGE(A43:E43)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="N43">
@@ -3920,19 +3915,19 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J44">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="K44">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L44">
-        <f>AVERAGE(A44:E44)</f>
+        <f t="shared" si="4"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="N44">
@@ -3962,19 +3957,19 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J45">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="K45">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L45">
-        <f>AVERAGE(A45:E45)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="N45">
@@ -4004,19 +3999,19 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1.0333333333333334</v>
       </c>
       <c r="J46">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.046242774566474E-2</v>
-      </c>
-      <c r="K46">
         <f t="shared" ca="1" si="2"/>
         <v>4.046242774566474E-2</v>
       </c>
+      <c r="K46">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.046242774566474E-2</v>
+      </c>
       <c r="L46">
-        <f>AVERAGE(A46:E46)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="N46">
@@ -4046,19 +4041,19 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="J47">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K47">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="L47">
-        <f>AVERAGE(A47:E47)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="N47">
@@ -4088,19 +4083,19 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.73333333333333328</v>
       </c>
       <c r="J48">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.3121387283236993E-2</v>
-      </c>
-      <c r="K48">
         <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
+      <c r="K48">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.3121387283236993E-2</v>
+      </c>
       <c r="L48">
-        <f>AVERAGE(A48:E48)</f>
+        <f t="shared" si="4"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="N48">
@@ -4130,19 +4125,19 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.5</v>
       </c>
       <c r="J49">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="K49">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L49">
-        <f>AVERAGE(A49:E49)</f>
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="N49">
@@ -4172,19 +4167,19 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.76666666666666672</v>
       </c>
       <c r="J50">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="K50">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="L50">
-        <f>AVERAGE(A50:E50)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="N50">
@@ -4214,61 +4209,61 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.7</v>
       </c>
       <c r="J51">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.4682080924855488E-2</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="4"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="N51">
+        <v>101</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K51">
+        <v>0.9</v>
+      </c>
+      <c r="J52">
         <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
-      <c r="L51">
-        <f>AVERAGE(A51:E51)</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="N51">
-        <v>101</v>
-      </c>
-      <c r="O51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
-      </c>
-      <c r="J52">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.4682080924855488E-2</v>
-      </c>
       <c r="K52">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="L52">
-        <f>AVERAGE(A52:E52)</f>
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="N52">
@@ -4298,19 +4293,19 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.73333333333333328</v>
       </c>
       <c r="J53">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="K53">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L53">
-        <f>AVERAGE(A53:E53)</f>
+        <f t="shared" si="4"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="N53">
@@ -4340,19 +4335,19 @@
         <v>1</v>
       </c>
       <c r="I54">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J54">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="K54">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L54">
-        <f>AVERAGE(A54:E54)</f>
+        <f t="shared" si="4"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="N54">
@@ -4382,19 +4377,19 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="J55">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="K55">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="L55">
-        <f>AVERAGE(A55:E55)</f>
+        <f t="shared" si="4"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="N55">
@@ -4424,19 +4419,19 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J56">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K56">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="L56">
-        <f>AVERAGE(A56:E56)</f>
+        <f t="shared" si="4"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="N56">
@@ -4466,19 +4461,19 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="J57">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K57">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="L57">
-        <f>AVERAGE(A57:E57)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N57">
@@ -4508,19 +4503,19 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.76666666666666672</v>
       </c>
       <c r="J58">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K58">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="L58">
-        <f>AVERAGE(A58:E58)</f>
+        <f t="shared" si="4"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="N58">
@@ -4550,19 +4545,19 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.76666666666666672</v>
       </c>
       <c r="J59">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.3121387283236993E-2</v>
-      </c>
-      <c r="K59">
         <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
+      <c r="K59">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.3121387283236993E-2</v>
+      </c>
       <c r="L59">
-        <f>AVERAGE(A59:E59)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="N59">
@@ -4592,19 +4587,19 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.6333333333333333</v>
       </c>
       <c r="J60">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K60">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L60">
-        <f>AVERAGE(A60:E60)</f>
+        <f t="shared" si="4"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="N60">
@@ -4634,19 +4629,19 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.9</v>
       </c>
       <c r="J61">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3.4682080924855488E-2</v>
       </c>
       <c r="K61">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L61">
-        <f>AVERAGE(A61:E61)</f>
+        <f t="shared" si="4"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="N61">
@@ -4676,19 +4671,19 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.73333333333333328</v>
       </c>
       <c r="J62">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="K62">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L62">
-        <f>AVERAGE(A62:E62)</f>
+        <f t="shared" si="4"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="N62">
@@ -4718,19 +4713,19 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J63">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.8901734104046242E-2</v>
-      </c>
-      <c r="K63">
         <f t="shared" ca="1" si="2"/>
         <v>2.8901734104046242E-2</v>
       </c>
+      <c r="K63">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.8901734104046242E-2</v>
+      </c>
       <c r="L63">
-        <f>AVERAGE(A63:E63)</f>
+        <f t="shared" si="4"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="N63">
@@ -4760,19 +4755,19 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="J64">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.2023121387283239E-2</v>
       </c>
       <c r="K64">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="L64">
-        <f>AVERAGE(A64:E64)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="N64">
@@ -4802,19 +4797,19 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.4</v>
       </c>
       <c r="J65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.7341040462427744E-2</v>
       </c>
       <c r="K65">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="L65">
-        <f>AVERAGE(A65:E65)</f>
+        <f t="shared" si="4"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="N65">
@@ -4844,19 +4839,19 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="J66">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="K66">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L66">
-        <f>AVERAGE(A66:E66)</f>
+        <f t="shared" si="4"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="N66">
@@ -4883,19 +4878,19 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I68" ca="1" si="3">AVERAGE(OFFSET($H$2,(ROW()-ROW($I$2))*30,,30,))</f>
+        <f t="shared" ref="I67:I68" ca="1" si="5">AVERAGE(OFFSET($H$2,(ROW()-ROW($I$2))*30,,30,))</f>
         <v>0.76666666666666672</v>
       </c>
       <c r="J67">
-        <f ca="1">AVERAGE(OFFSET($G$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ref="J67:J69" ca="1" si="6">AVERAGE(OFFSET($G$2,(ROW()-ROW($J$2))*173,,173,))</f>
         <v>4.6242774566473986E-2</v>
       </c>
       <c r="K67">
-        <f ca="1">AVERAGE(OFFSET($F$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ref="K67:K69" ca="1" si="7">AVERAGE(OFFSET($F$2,(ROW()-ROW($K$2))*173,,173,))</f>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="L67">
-        <f>AVERAGE(A67:E67)</f>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
       <c r="N67">
@@ -4922,19 +4917,19 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="J68">
-        <f ca="1">AVERAGE(OFFSET($G$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>2.3121387283236993E-2</v>
       </c>
       <c r="K68">
-        <f ca="1">AVERAGE(OFFSET($F$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>2.8901734104046242E-2</v>
       </c>
       <c r="L68">
-        <f>AVERAGE(A68:E68)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="N68">
@@ -4962,15 +4957,15 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="J69">
-        <f ca="1">AVERAGE(OFFSET($G$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>1.1560693641618497E-2</v>
       </c>
       <c r="K69">
-        <f ca="1">AVERAGE(OFFSET($F$2,(ROW()-ROW($I$2))*173,,173,))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>5.7803468208092483E-3</v>
       </c>
       <c r="L69">
-        <f>AVERAGE(A69:E69)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N69">

</xml_diff>